<commit_message>
Added test cases to the latest VB version
</commit_message>
<xml_diff>
--- a/REFramework/contentFiles/any/any/pt0/VisualBasic/Tests/Tests.xlsx
+++ b/REFramework/contentFiles/any/any/pt0/VisualBasic/Tests/Tests.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27B09E86-E7F7-40F4-8A4B-0931C3A3679A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{27B09E86-E7F7-40F4-8A4B-0931C3A3679A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E1911DC-185D-43E5-B71F-2609E8CB9E61}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="9">
   <si>
     <t>WorkflowFile</t>
   </si>
@@ -395,7 +395,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
@@ -488,9 +490,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
@@ -514,6 +518,70 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D1" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <phoneticPr fontId="3"/>

</xml_diff>

<commit_message>
Renamed GeneralTestCase and added KillAllProcess to variation file
</commit_message>
<xml_diff>
--- a/REFramework/contentFiles/any/any/pt0/VisualBasic/Tests/Tests.xlsx
+++ b/REFramework/contentFiles/any/any/pt0/VisualBasic/Tests/Tests.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{27B09E86-E7F7-40F4-8A4B-0931C3A3679A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E1911DC-185D-43E5-B71F-2609E8CB9E61}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{27B09E86-E7F7-40F4-8A4B-0931C3A3679A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E16D29D-363D-4A14-96A7-2A4C4F7A038F}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4270" yWindow="-14510" windowWidth="25820" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="10">
   <si>
     <t>WorkflowFile</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>SystemException</t>
+  </si>
+  <si>
+    <t>Framework\KillAllProcesses.xaml</t>
   </si>
 </sst>
 </file>
@@ -393,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -473,6 +476,14 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>1</v>
       </c>
     </row>
@@ -490,10 +501,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -582,6 +593,14 @@
         <v>1</v>
       </c>
     </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D1" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <phoneticPr fontId="3"/>

</xml_diff>